<commit_message>
fix: update data and program
</commit_message>
<xml_diff>
--- a/data_temp/tahap6_hasil_perbandingan.xlsx
+++ b/data_temp/tahap6_hasil_perbandingan.xlsx
@@ -513,14 +513,14 @@
         </is>
       </c>
       <c r="B2" s="3" t="n">
-        <v>0.04</v>
+        <v>0.23</v>
       </c>
       <c r="C2" s="3" t="n">
-        <v>1.55</v>
+        <v>14.89</v>
       </c>
       <c r="D2" s="3" t="inlineStr">
         <is>
-          <t>3775.0%</t>
+          <t>6373.9%</t>
         </is>
       </c>
     </row>
@@ -531,14 +531,14 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>203</v>
+        <v>4</v>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>2437.5%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -549,14 +549,14 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.6667</v>
+        <v>0.6116</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.908</v>
+        <v>0.6116</v>
       </c>
       <c r="D4" s="3" t="inlineStr">
         <is>
-          <t>36.2%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -567,14 +567,14 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>2.2222</v>
+        <v>1.0052</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>6.8247</v>
+        <v>1.0052</v>
       </c>
       <c r="D5" s="3" t="inlineStr">
         <is>
-          <t>207.1%</t>
+          <t>0.0%</t>
         </is>
       </c>
     </row>
@@ -585,10 +585,10 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D6" s="3" t="inlineStr">
         <is>
@@ -603,10 +603,10 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="C7" s="3" t="n">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D7" s="3" t="inlineStr">
         <is>

</xml_diff>